<commit_message>
updating calculations and tables
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
+++ b/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="0" windowWidth="23840" windowHeight="15740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1060" yWindow="0" windowWidth="23840" windowHeight="15740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data summary" sheetId="1" r:id="rId1"/>
     <sheet name="Semantic correctness" sheetId="2" r:id="rId2"/>
     <sheet name="Syntactic correctness" sheetId="4" r:id="rId3"/>
+    <sheet name="Overall correctness" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Total count</t>
   </si>
@@ -123,6 +124,21 @@
   </si>
   <si>
     <t># minor correction</t>
+  </si>
+  <si>
+    <t>note- the three tables below are the same as the table to the right</t>
+  </si>
+  <si>
+    <t>This is the summary data:</t>
+  </si>
+  <si>
+    <t>total incorrect</t>
+  </si>
+  <si>
+    <t>perent incorrect</t>
+  </si>
+  <si>
+    <t># correct (semantic correctness)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +187,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -186,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -306,8 +329,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -398,12 +487,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -429,8 +535,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="110">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -475,6 +602,16 @@
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -519,6 +656,16 @@
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -948,362 +1095,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="47" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="46" thickBot="1">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="33"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="I2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L2" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:12" s="2" customFormat="1">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="26"/>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$472</f>
         <v>430</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$479</f>
         <v>466</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$476</f>
         <v>36</v>
       </c>
-      <c r="H2" s="4">
-        <f>G2/F2</f>
+      <c r="H3" s="3">
+        <f>G3/F3</f>
         <v>7.7253218884120178E-2</v>
       </c>
-      <c r="I2">
-        <f>E2-J2</f>
+      <c r="I3">
+        <f>E3-J3</f>
         <v>416</v>
       </c>
-      <c r="J2">
+      <c r="J3">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$472</f>
         <v>14</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$476</f>
         <v>152</v>
       </c>
-      <c r="L2" s="4">
-        <f>K2/E2</f>
+      <c r="L3" s="3">
+        <f>K3/E3</f>
         <v>0.35348837209302325</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="28">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$472</f>
         <v>430</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <f>'[1]Organisms- POST'!$E$145</f>
         <v>55</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <f>'[1]Organisms- POST'!$E$152</f>
         <v>139</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <f>'[1]Organisms- POST'!$E$149</f>
         <v>84</v>
       </c>
-      <c r="H3" s="4">
-        <f>G3/F3</f>
+      <c r="H4" s="3">
+        <f>G4/F4</f>
         <v>0.60431654676258995</v>
       </c>
-      <c r="I3">
-        <f>E3-J3</f>
+      <c r="I4">
+        <f>E4-J4</f>
         <v>48</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <f>'[1]Organisms- POST'!$G$145</f>
         <v>7</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <f>'[1]Organisms- POST'!$G$149</f>
         <v>8</v>
       </c>
-      <c r="L3" s="4">
-        <f t="shared" ref="L3:L6" si="0">K3/E3</f>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L7" si="0">K4/E4</f>
         <v>0.14545454545454545</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="28">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$479</f>
         <v>466</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f>'[1]Software- POST C v NC'!$E$106</f>
         <v>78</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <f>'[1]Software- POST C v NC'!$E$113</f>
         <v>101</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <f>'[1]Software- POST C v NC'!$E$110</f>
         <v>22</v>
       </c>
-      <c r="H4" s="4">
-        <f>G4/F4</f>
+      <c r="H5" s="3">
+        <f>G5/F5</f>
         <v>0.21782178217821782</v>
       </c>
-      <c r="I4">
-        <f>E4-J4</f>
+      <c r="I5">
+        <f>E5-J5</f>
         <v>77</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <f>'[1]Software- POST C v NC'!$G$106</f>
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <f>'[1]Software- POST C v NC'!$G$110</f>
         <v>26</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L5" s="3">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="28">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$476</f>
         <v>36</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="D6" s="1"/>
+      <c r="H6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <f>B3-B7</f>
+      <c r="B7" s="28">
+        <f>B4-B8</f>
         <v>416</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
-        <f>SUM(E2:E4)</f>
+      <c r="E7" s="23">
+        <f>SUM(E3:E5)</f>
         <v>563</v>
       </c>
-      <c r="F6">
-        <f>SUM(F2:F4)</f>
+      <c r="F7" s="23">
+        <f>SUM(F3:F5)</f>
         <v>706</v>
       </c>
-      <c r="G6">
-        <f>SUM(G2:G4)</f>
+      <c r="G7" s="23">
+        <f>SUM(G3:G5)</f>
         <v>142</v>
       </c>
-      <c r="H6" s="4">
-        <f>G6/F6</f>
+      <c r="H7" s="24">
+        <f>G7/F7</f>
         <v>0.20113314447592068</v>
       </c>
-      <c r="I6">
-        <f>SUM(I2:I4)</f>
+      <c r="I7" s="23">
+        <f>SUM(I3:I5)</f>
         <v>541</v>
       </c>
-      <c r="J6">
-        <f>SUM(J2:J4)</f>
+      <c r="J7" s="23">
+        <f>SUM(J3:J5)</f>
         <v>22</v>
       </c>
-      <c r="K6">
-        <f>SUM(K2:K4)</f>
+      <c r="K7" s="23">
+        <f>SUM(K3:K5)</f>
         <v>186</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L7" s="24">
         <f t="shared" si="0"/>
         <v>0.33037300177619894</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="28">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$472</f>
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
+      <c r="A9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="31">
         <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$476</f>
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:12" ht="16" thickBot="1"/>
+    <row r="11" spans="1:12" ht="16" thickBot="1">
+      <c r="A11" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="33"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="28">
         <f>'[1]Organisms- POST'!$E$145</f>
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="28">
         <f>'[1]Organisms- POST'!$E$152</f>
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" t="s">
+    <row r="14" spans="1:12">
+      <c r="A14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="28">
         <f>'[1]Organisms- POST'!$E$149</f>
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
+    <row r="15" spans="1:12">
+      <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B14">
-        <f>B11-B15</f>
+      <c r="B15" s="28">
+        <f>B12-B16</f>
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="28">
         <f>'[1]Organisms- POST'!$G$145</f>
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" ht="16" thickBot="1">
+      <c r="A17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="31">
         <f>'[1]Organisms- POST'!$G$149</f>
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:2" ht="16" thickBot="1"/>
+    <row r="19" spans="1:2" ht="16" thickBot="1">
+      <c r="A19" s="32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="33"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="28">
         <f>'[1]Software- POST C v NC'!$E$106</f>
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="28">
         <f>'[1]Software- POST C v NC'!$E$113</f>
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="28">
         <f>'[1]Software- POST C v NC'!$E$110</f>
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22">
-        <f>B19-B23</f>
+      <c r="B23" s="28">
+        <f>B20-B24</f>
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B23">
+      <c r="B24" s="28">
         <f>'[1]Software- POST C v NC'!$G$106</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" ht="16" thickBot="1">
+      <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="31">
         <f>'[1]Software- POST C v NC'!$G$110</f>
         <v>26</v>
       </c>
@@ -1324,7 +1489,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D14"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1335,19 +1500,19 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="45">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1356,22 +1521,22 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <f>'Data summary'!B6</f>
+        <f>'Data summary'!B7</f>
         <v>416</v>
       </c>
       <c r="C3">
-        <f>'Data summary'!B7</f>
+        <f>'Data summary'!B8</f>
         <v>14</v>
       </c>
       <c r="D3">
-        <f>'Data summary'!B3</f>
+        <f>'Data summary'!B4</f>
         <v>430</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>B3/D3</f>
         <v>0.96744186046511627</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <f>C3/D3</f>
         <v>3.255813953488372E-2</v>
       </c>
@@ -1381,22 +1546,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <f>'Data summary'!B14</f>
+        <f>'Data summary'!B15</f>
         <v>48</v>
       </c>
       <c r="C4">
-        <f>'Data summary'!B15</f>
+        <f>'Data summary'!B16</f>
         <v>7</v>
       </c>
       <c r="D4">
-        <f>'Data summary'!B11</f>
+        <f>'Data summary'!B12</f>
         <v>55</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <f t="shared" ref="E4:E5" si="0">B4/D4</f>
         <v>0.87272727272727268</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <f>C4/D4</f>
         <v>0.12727272727272726</v>
       </c>
@@ -1406,32 +1571,32 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <f>'Data summary'!B22</f>
+        <f>'Data summary'!B23</f>
         <v>77</v>
       </c>
       <c r="C5">
-        <f>'Data summary'!B23</f>
+        <f>'Data summary'!B24</f>
         <v>1</v>
       </c>
       <c r="D5">
-        <f>'Data summary'!B19</f>
+        <f>'Data summary'!B20</f>
         <v>78</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>0.98717948717948723</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f>C5/D5</f>
         <v>1.282051282051282E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -1446,15 +1611,15 @@
         <f>SUM(D3:D5)</f>
         <v>563</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f>B7/D7</f>
         <v>0.96092362344582594</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f>C7/D7</f>
         <v>3.9076376554174071E-2</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1462,81 +1627,81 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="31" thickBot="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16" thickTop="1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <f>C3</f>
         <v>14</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <f>D3</f>
         <v>430</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <f>F3</f>
         <v>3.255813953488372E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <f>C4</f>
         <v>7</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>D4</f>
         <v>55</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f>F4</f>
         <v>0.12727272727272726</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" thickBot="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <f>C5</f>
         <v>1</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <f>D5</f>
         <v>78</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <f>F5</f>
         <v>1.282051282051282E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" thickBot="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <f>SUM(B11:B13)</f>
         <v>22</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <f>SUM(C11:C13)</f>
         <v>563</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>4.6181172291296625E-2</v>
       </c>
     </row>
@@ -1555,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -1567,83 +1732,253 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="31" thickBot="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickTop="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10">
-        <f>'Data summary'!K2</f>
+      <c r="B3" s="9">
+        <f>'Data summary'!K3</f>
         <v>152</v>
       </c>
-      <c r="C3" s="10">
-        <f>'Data summary'!E2</f>
+      <c r="C3" s="9">
+        <f>'Data summary'!E3</f>
         <v>430</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <f>B3/C3</f>
         <v>0.35348837209302325</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10">
-        <f>'Data summary'!K3</f>
+      <c r="B4" s="9">
+        <f>'Data summary'!K4</f>
         <v>8</v>
       </c>
-      <c r="C4" s="10">
-        <f>'Data summary'!E3</f>
+      <c r="C4" s="9">
+        <f>'Data summary'!E4</f>
         <v>55</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f>B4/C4</f>
         <v>0.14545454545454545</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="19">
-        <f>'Data summary'!K4</f>
+      <c r="B5" s="18">
+        <f>'Data summary'!K5</f>
         <v>26</v>
       </c>
-      <c r="C5" s="19">
-        <f>'Data summary'!E4</f>
+      <c r="C5" s="18">
+        <f>'Data summary'!E5</f>
         <v>78</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="19">
         <f>B5/C5</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <f>SUM(B3:B5)</f>
         <v>186</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <f>SUM(C3:C5)</f>
         <v>563</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f>B6/C6</f>
         <v>0.33037300177619894</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="45">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22" t="str">
+        <f>'Data summary'!E2</f>
+        <v>Resources with RRID</v>
+      </c>
+      <c r="C2" s="22" t="str">
+        <f>'Data summary'!I2</f>
+        <v># correct (semantic correctness)</v>
+      </c>
+      <c r="D2" s="22" t="str">
+        <f>'Data summary'!J2</f>
+        <v># incorrect (semantic correctness)</v>
+      </c>
+      <c r="E2" s="22" t="str">
+        <f>'Data summary'!K2</f>
+        <v>minor correction (syntactic correctness)</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="str">
+        <f>'Data summary'!D3</f>
+        <v>Antibodies</v>
+      </c>
+      <c r="B3">
+        <f>'Data summary'!E3</f>
+        <v>430</v>
+      </c>
+      <c r="C3">
+        <f>'Data summary'!I3</f>
+        <v>416</v>
+      </c>
+      <c r="D3">
+        <f>'Data summary'!J3</f>
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <f>'Data summary'!K3</f>
+        <v>152</v>
+      </c>
+      <c r="F3">
+        <f>SUM(D3:E3)</f>
+        <v>166</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/B3</f>
+        <v>0.38604651162790699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="str">
+        <f>'Data summary'!D4</f>
+        <v>Organisms</v>
+      </c>
+      <c r="B4">
+        <f>'Data summary'!E4</f>
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <f>'Data summary'!I4</f>
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <f>'Data summary'!J4</f>
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <f>'Data summary'!K4</f>
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <f>SUM(D4:E4)</f>
+        <v>15</v>
+      </c>
+      <c r="G4" s="3">
+        <f>F4/B4</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="str">
+        <f>'Data summary'!D5</f>
+        <v>Software</v>
+      </c>
+      <c r="B5">
+        <f>'Data summary'!E5</f>
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <f>'Data summary'!I5</f>
+        <v>77</v>
+      </c>
+      <c r="D5">
+        <f>'Data summary'!J5</f>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>'Data summary'!K5</f>
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <f>SUM(D5:E5)</f>
+        <v>27</v>
+      </c>
+      <c r="G5" s="3">
+        <f>F5/B5</f>
+        <v>0.34615384615384615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="23" t="str">
+        <f>'Data summary'!D7</f>
+        <v>Total</v>
+      </c>
+      <c r="B7" s="23">
+        <f>'Data summary'!E7</f>
+        <v>563</v>
+      </c>
+      <c r="C7" s="23">
+        <f>'Data summary'!I7</f>
+        <v>541</v>
+      </c>
+      <c r="D7" s="23">
+        <f>'Data summary'!J7</f>
+        <v>22</v>
+      </c>
+      <c r="E7" s="23">
+        <f>'Data summary'!K7</f>
+        <v>186</v>
+      </c>
+      <c r="F7" s="23">
+        <f>SUM(D7:E7)</f>
+        <v>208</v>
+      </c>
+      <c r="G7" s="24">
+        <f>F7/B7</f>
+        <v>0.369449378330373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Figure3 analysis in v10 of the analysis spreadsheet. This is now replaced with the figure in the SummaryCalculations spreadsheet
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
+++ b/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Total count</t>
   </si>
@@ -144,10 +144,37 @@
     <t>Summary data for figure</t>
   </si>
   <si>
-    <t>Incorrect resource (percent)</t>
-  </si>
-  <si>
-    <t>Overall perent incorrect</t>
+    <t>Correct resource (percent)</t>
+  </si>
+  <si>
+    <t>Correct syntax PERCENT</t>
+  </si>
+  <si>
+    <t>Correct syntax</t>
+  </si>
+  <si>
+    <t>Percentage with correct syntax</t>
+  </si>
+  <si>
+    <t>Overall percent incorrect</t>
+  </si>
+  <si>
+    <t>Total correct</t>
+  </si>
+  <si>
+    <t>Summary Table</t>
+  </si>
+  <si>
+    <t>Total number of Resources with RRID</t>
+  </si>
+  <si>
+    <t>Number of Resources with Correct RRID</t>
+  </si>
+  <si>
+    <t>Number of Resource with Correct Syntax</t>
+  </si>
+  <si>
+    <t>Total number of Correct Resources - Overall</t>
   </si>
 </sst>
 </file>
@@ -405,9 +432,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="136">
+  <cellStyleXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -595,7 +670,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="136">
+  <cellStyles count="184">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -663,6 +738,30 @@
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -730,6 +829,30 @@
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -781,13 +904,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0325581395348837</c:v>
+                  <c:v>0.967441860465116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.353488372093023</c:v>
+                  <c:v>0.646511627906977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.386046511627907</c:v>
+                  <c:v>0.613953488372093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,13 +938,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.127272727272727</c:v>
+                  <c:v>0.872727272727273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.145454545454545</c:v>
+                  <c:v>0.854545454545454</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.272727272727273</c:v>
+                  <c:v>0.727272727272727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,13 +972,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0128205128205128</c:v>
+                  <c:v>0.987179487179487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.346153846153846</c:v>
+                  <c:v>0.653846153846154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -908,7 +1031,7 @@
         <c:axId val="2143734376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.5"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -942,16 +1065,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1394,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1408,7 +1531,7 @@
     <col min="11" max="11" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="47" thickBot="1">
+    <row r="1" spans="1:15" ht="47" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -1416,7 +1539,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="46" thickBot="1">
+    <row r="2" spans="1:15" ht="46" thickBot="1">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -1452,8 +1575,11 @@
       <c r="N2" s="22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="2" customFormat="1">
+      <c r="O2" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -1501,8 +1627,12 @@
         <f>M3/E3</f>
         <v>0.38604651162790699</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="2">
+        <f>E3-J3-K3</f>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -1553,8 +1683,12 @@
         <f>M4/E4</f>
         <v>0.27272727272727271</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="2">
+        <f>E4-J4-K4</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="29" t="s">
         <v>7</v>
       </c>
@@ -1605,8 +1739,12 @@
         <f>M5/E5</f>
         <v>0.34615384615384615</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="2">
+        <f>E5-J5-K5</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
@@ -1618,7 +1756,7 @@
       <c r="H6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
@@ -1669,8 +1807,12 @@
         <f>M7/E7</f>
         <v>0.369449378330373</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7">
+        <f>SUM(O3:O5)</f>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -1679,7 +1821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" thickBot="1">
+    <row r="9" spans="1:15" ht="16" thickBot="1">
       <c r="A9" s="30" t="s">
         <v>6</v>
       </c>
@@ -1688,12 +1830,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" thickBot="1">
+    <row r="10" spans="1:15" ht="16" thickBot="1">
       <c r="D10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="46" thickBot="1">
+    <row r="11" spans="1:15" ht="46" thickBot="1">
       <c r="A11" s="32" t="s">
         <v>8</v>
       </c>
@@ -1702,13 +1844,13 @@
         <v>39</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="27" t="s">
         <v>9</v>
       </c>
@@ -1720,19 +1862,19 @@
         <v>2</v>
       </c>
       <c r="E12" s="36">
-        <f>'Semantic correctness'!D11</f>
-        <v>3.255813953488372E-2</v>
+        <f>'Semantic correctness'!E3</f>
+        <v>0.96744186046511627</v>
       </c>
       <c r="F12" s="36">
-        <f>L3</f>
-        <v>0.35348837209302325</v>
+        <f>'Syntactic correctness'!F3</f>
+        <v>0.64651162790697669</v>
       </c>
       <c r="G12" s="36">
-        <f>N3</f>
-        <v>0.38604651162790699</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <f>O3/E3</f>
+        <v>0.61395348837209307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="29" t="s">
         <v>10</v>
       </c>
@@ -1744,19 +1886,19 @@
         <v>8</v>
       </c>
       <c r="E13" s="36">
-        <f>'Semantic correctness'!D12</f>
-        <v>0.12727272727272726</v>
+        <f>'Semantic correctness'!E4</f>
+        <v>0.87272727272727268</v>
       </c>
       <c r="F13" s="36">
-        <f>L4</f>
-        <v>0.14545454545454545</v>
+        <f>'Syntactic correctness'!F4</f>
+        <v>0.8545454545454545</v>
       </c>
       <c r="G13" s="36">
-        <f>N4</f>
-        <v>0.27272727272727271</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <f>O4/E4</f>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="29" t="s">
         <v>11</v>
       </c>
@@ -1768,19 +1910,19 @@
         <v>17</v>
       </c>
       <c r="E14" s="36">
-        <f>'Semantic correctness'!D13</f>
-        <v>1.282051282051282E-2</v>
+        <f>'Semantic correctness'!E5</f>
+        <v>0.98717948717948723</v>
       </c>
       <c r="F14" s="36">
-        <f>L5</f>
-        <v>0.33333333333333331</v>
+        <f>'Syntactic correctness'!F5</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G14" s="36">
-        <f>N5</f>
-        <v>0.34615384615384615</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <f>O5/E5</f>
+        <v>0.65384615384615385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
@@ -1792,19 +1934,19 @@
         <v>18</v>
       </c>
       <c r="E15" s="37">
-        <f>'Semantic correctness'!D14</f>
-        <v>4.6181172291296625E-2</v>
+        <f>'Semantic correctness'!E7</f>
+        <v>0.96092362344582594</v>
       </c>
       <c r="F15" s="37">
-        <f>L7</f>
-        <v>0.33037300177619894</v>
+        <f>'Syntactic correctness'!F6</f>
+        <v>0.66962699822380112</v>
       </c>
       <c r="G15" s="37">
-        <f>N7</f>
-        <v>0.369449378330373</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <f>O7/E7</f>
+        <v>0.63055062166962694</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="29" t="s">
         <v>5</v>
       </c>
@@ -1813,7 +1955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" thickBot="1">
+    <row r="17" spans="1:8" ht="31" thickBot="1">
       <c r="A17" s="30" t="s">
         <v>6</v>
       </c>
@@ -1821,15 +1963,50 @@
         <f>'[1]Organisms- POST'!$G$149</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="16" thickBot="1"/>
-    <row r="19" spans="1:2" ht="16" thickBot="1">
+      <c r="D17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="76" thickBot="1">
+      <c r="E18" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="33"/>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <f>I3</f>
+        <v>416</v>
+      </c>
+      <c r="F19">
+        <f>'Syntactic correctness'!E3</f>
+        <v>278</v>
+      </c>
+      <c r="G19">
+        <f>O3</f>
+        <v>264</v>
+      </c>
+      <c r="H19">
+        <f>E3</f>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="27" t="s">
         <v>12</v>
       </c>
@@ -1837,8 +2014,27 @@
         <f>'[1]Software- POST C v NC'!$E$106</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <f>I4</f>
+        <v>48</v>
+      </c>
+      <c r="F20">
+        <f>'Syntactic correctness'!E4</f>
+        <v>47</v>
+      </c>
+      <c r="G20">
+        <f>O4</f>
+        <v>40</v>
+      </c>
+      <c r="H20">
+        <f>E4</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="29" t="s">
         <v>13</v>
       </c>
@@ -1846,8 +2042,27 @@
         <f>'[1]Software- POST C v NC'!$E$113</f>
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <f>I5</f>
+        <v>77</v>
+      </c>
+      <c r="F21">
+        <f>'Syntactic correctness'!E5</f>
+        <v>52</v>
+      </c>
+      <c r="G21">
+        <f>O5</f>
+        <v>51</v>
+      </c>
+      <c r="H21">
+        <f>E5</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="29" t="s">
         <v>14</v>
       </c>
@@ -1855,8 +2070,27 @@
         <f>'[1]Software- POST C v NC'!$E$110</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="23">
+        <f>SUM(E19:E21)</f>
+        <v>541</v>
+      </c>
+      <c r="F22" s="23">
+        <f>'Syntactic correctness'!E6</f>
+        <v>377</v>
+      </c>
+      <c r="G22" s="23">
+        <f>SUM(G19:G21)</f>
+        <v>355</v>
+      </c>
+      <c r="H22" s="23">
+        <f>SUM(H19:H21)</f>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="29" t="s">
         <v>4</v>
       </c>
@@ -1864,8 +2098,20 @@
         <f>B20-B24</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="E23" s="3">
+        <f>E22/$H$22</f>
+        <v>0.96092362344582594</v>
+      </c>
+      <c r="F23" s="3">
+        <f>F22/$H$22</f>
+        <v>0.66962699822380112</v>
+      </c>
+      <c r="G23" s="3">
+        <f>G22/$H$22</f>
+        <v>0.63055062166962694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="29" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" thickBot="1">
+    <row r="25" spans="1:8" ht="16" thickBot="1">
       <c r="A25" s="30" t="s">
         <v>6</v>
       </c>
@@ -1900,7 +2146,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1969,7 +2215,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E5" si="0">B4/D4</f>
+        <f>B4/D4</f>
         <v>0.87272727272727268</v>
       </c>
       <c r="F4" s="3">
@@ -1994,7 +2240,7 @@
         <v>78</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E4:E5" si="0">B5/D5</f>
         <v>0.98717948717948723</v>
       </c>
       <c r="F5" s="3">
@@ -2075,7 +2321,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="9">
-        <f t="shared" si="1"/>
+        <f>D4</f>
         <v>55</v>
       </c>
       <c r="D12" s="10">
@@ -2129,20 +2375,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F6" sqref="F3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31" thickBot="1">
+    <row r="2" spans="1:6" ht="31" thickBot="1">
       <c r="A2" s="15"/>
       <c r="B2" s="17" t="s">
         <v>32</v>
@@ -2153,8 +2399,14 @@
       <c r="D2" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" thickTop="1">
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" thickTop="1">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
@@ -2170,8 +2422,16 @@
         <f>B3/C3</f>
         <v>0.35348837209302325</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <f>C3-B3</f>
+        <v>278</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3/C3</f>
+        <v>0.64651162790697669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -2187,8 +2447,16 @@
         <f>B4/C4</f>
         <v>0.14545454545454545</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1">
+      <c r="E4">
+        <f>C4-B4</f>
+        <v>47</v>
+      </c>
+      <c r="F4" s="3">
+        <f>E4/C4</f>
+        <v>0.8545454545454545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -2204,8 +2472,16 @@
         <f>B5/C5</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1">
+      <c r="E5">
+        <f>C5-B5</f>
+        <v>52</v>
+      </c>
+      <c r="F5" s="3">
+        <f>E5/C5</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
@@ -2220,6 +2496,14 @@
       <c r="D6" s="14">
         <f>B6/C6</f>
         <v>0.33037300177619894</v>
+      </c>
+      <c r="E6">
+        <f>C6-B6</f>
+        <v>377</v>
+      </c>
+      <c r="F6" s="3">
+        <f>E6/C6</f>
+        <v>0.66962699822380112</v>
       </c>
     </row>
   </sheetData>
@@ -2238,7 +2522,7 @@
   <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
minor edits to the raw data and updated analysis
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
+++ b/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Total count</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Total number of Correct Resources - Overall</t>
+  </si>
+  <si>
+    <t>Tools</t>
   </si>
 </sst>
 </file>
@@ -904,13 +907,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.967441860465116</c:v>
+                  <c:v>0.959287531806616</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.646511627906977</c:v>
+                  <c:v>0.575063613231552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.613953488372093</c:v>
+                  <c:v>0.534351145038168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,7 +962,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Software</c:v>
+                  <c:v>Tools</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1101,12 +1104,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Antibodies-PRE"/>
-      <sheetName val="Antibody-POST 1st vs 2nd Abs"/>
+      <sheetName val="Antibody-POST"/>
       <sheetName val="Organisms-PRE"/>
       <sheetName val="Organisms- POST"/>
       <sheetName val="Software-PRE"/>
       <sheetName val="Software- POST C v NC"/>
-      <sheetName val="Figure 3"/>
       <sheetName val="Figure 4"/>
       <sheetName val="binary significance test"/>
       <sheetName val="Correct usage"/>
@@ -1115,48 +1117,48 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="472">
-          <cell r="E472">
-            <v>430</v>
+        <row r="471">
+          <cell r="H471">
+            <v>393</v>
           </cell>
-          <cell r="G472">
-            <v>14</v>
+          <cell r="J471">
+            <v>16</v>
           </cell>
         </row>
-        <row r="476">
-          <cell r="E476">
+        <row r="475">
+          <cell r="H475">
             <v>36</v>
           </cell>
-          <cell r="G476">
-            <v>152</v>
+          <cell r="J475">
+            <v>167</v>
           </cell>
         </row>
-        <row r="479">
-          <cell r="E479">
-            <v>466</v>
+        <row r="478">
+          <cell r="H478">
+            <v>465</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="145">
-          <cell r="E145">
+          <cell r="H145">
             <v>55</v>
           </cell>
-          <cell r="G145">
+          <cell r="J145">
             <v>7</v>
           </cell>
         </row>
         <row r="149">
-          <cell r="E149">
+          <cell r="H149">
             <v>84</v>
           </cell>
-          <cell r="G149">
+          <cell r="J149">
             <v>8</v>
           </cell>
         </row>
         <row r="152">
-          <cell r="E152">
+          <cell r="H152">
             <v>139</v>
           </cell>
         </row>
@@ -1164,23 +1166,23 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="106">
-          <cell r="E106">
+          <cell r="H106">
             <v>78</v>
           </cell>
-          <cell r="G106">
+          <cell r="J106">
             <v>1</v>
           </cell>
         </row>
         <row r="110">
-          <cell r="E110">
+          <cell r="H110">
             <v>22</v>
           </cell>
-          <cell r="G110">
+          <cell r="J110">
             <v>26</v>
           </cell>
         </row>
         <row r="113">
-          <cell r="E113">
+          <cell r="H113">
             <v>101</v>
           </cell>
         </row>
@@ -1189,7 +1191,6 @@
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1519,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1588,48 +1589,48 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$472</f>
-        <v>430</v>
+        <f>'[1]Antibody-POST'!$H$471</f>
+        <v>393</v>
       </c>
       <c r="F3">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$479</f>
-        <v>466</v>
+        <f>'[1]Antibody-POST'!$H$478</f>
+        <v>465</v>
       </c>
       <c r="G3">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$476</f>
+        <f>'[1]Antibody-POST'!$H$475</f>
         <v>36</v>
       </c>
       <c r="H3" s="3">
         <f>G3/F3</f>
-        <v>7.7253218884120178E-2</v>
+        <v>7.7419354838709681E-2</v>
       </c>
       <c r="I3">
         <f>E3-J3</f>
-        <v>416</v>
+        <v>377</v>
       </c>
       <c r="J3">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$472</f>
-        <v>14</v>
+        <f>'[1]Antibody-POST'!$J$471</f>
+        <v>16</v>
       </c>
       <c r="K3">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$476</f>
-        <v>152</v>
+        <f>'[1]Antibody-POST'!$J$475</f>
+        <v>167</v>
       </c>
       <c r="L3" s="3">
         <f>K3/E3</f>
-        <v>0.35348837209302325</v>
+        <v>0.42493638676844786</v>
       </c>
       <c r="M3">
         <f>SUM(J3:K3)</f>
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="N3" s="3">
         <f>M3/E3</f>
-        <v>0.38604651162790699</v>
+        <v>0.46564885496183206</v>
       </c>
       <c r="O3" s="2">
         <f>E3-J3-K3</f>
-        <v>264</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1637,22 +1638,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="28">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$472</f>
-        <v>430</v>
+        <f>'[1]Antibody-POST'!$H$471</f>
+        <v>393</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4">
-        <f>'[1]Organisms- POST'!$E$145</f>
+        <f>'[1]Organisms- POST'!$H$145</f>
         <v>55</v>
       </c>
       <c r="F4">
-        <f>'[1]Organisms- POST'!$E$152</f>
+        <f>'[1]Organisms- POST'!$H$152</f>
         <v>139</v>
       </c>
       <c r="G4">
-        <f>'[1]Organisms- POST'!$E$149</f>
+        <f>'[1]Organisms- POST'!$H$149</f>
         <v>84</v>
       </c>
       <c r="H4" s="3">
@@ -1664,11 +1665,11 @@
         <v>48</v>
       </c>
       <c r="J4">
-        <f>'[1]Organisms- POST'!$G$145</f>
+        <f>'[1]Organisms- POST'!$J$145</f>
         <v>7</v>
       </c>
       <c r="K4">
-        <f>'[1]Organisms- POST'!$G$149</f>
+        <f>'[1]Organisms- POST'!$J$149</f>
         <v>8</v>
       </c>
       <c r="L4" s="3">
@@ -1693,22 +1694,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="28">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$479</f>
-        <v>466</v>
+        <f>'[1]Antibody-POST'!$H$478</f>
+        <v>465</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E5">
-        <f>'[1]Software- POST C v NC'!$E$106</f>
+        <f>'[1]Software- POST C v NC'!$H$106</f>
         <v>78</v>
       </c>
       <c r="F5">
-        <f>'[1]Software- POST C v NC'!$E$113</f>
+        <f>'[1]Software- POST C v NC'!$H$113</f>
         <v>101</v>
       </c>
       <c r="G5">
-        <f>'[1]Software- POST C v NC'!$E$110</f>
+        <f>'[1]Software- POST C v NC'!$H$110</f>
         <v>22</v>
       </c>
       <c r="H5" s="3">
@@ -1720,11 +1721,11 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <f>'[1]Software- POST C v NC'!$G$106</f>
+        <f>'[1]Software- POST C v NC'!$J$106</f>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>'[1]Software- POST C v NC'!$G$110</f>
+        <f>'[1]Software- POST C v NC'!$J$110</f>
         <v>26</v>
       </c>
       <c r="L5" s="3">
@@ -1749,7 +1750,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="28">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$E$476</f>
+        <f>'[1]Antibody-POST'!$H$475</f>
         <v>36</v>
       </c>
       <c r="D6" s="1"/>
@@ -1762,18 +1763,18 @@
       </c>
       <c r="B7" s="28">
         <f>B4-B8</f>
-        <v>416</v>
+        <v>377</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="23">
         <f>SUM(E3:E5)</f>
-        <v>563</v>
+        <v>526</v>
       </c>
       <c r="F7" s="23">
         <f>SUM(F3:F5)</f>
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G7" s="23">
         <f>SUM(G3:G5)</f>
@@ -1781,35 +1782,35 @@
       </c>
       <c r="H7" s="24">
         <f>G7/F7</f>
-        <v>0.20113314447592068</v>
+        <v>0.20141843971631207</v>
       </c>
       <c r="I7" s="23">
         <f>SUM(I3:I5)</f>
-        <v>541</v>
+        <v>502</v>
       </c>
       <c r="J7" s="23">
         <f>SUM(J3:J5)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K7" s="23">
         <f>SUM(K3:K5)</f>
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="L7" s="24">
         <f t="shared" si="0"/>
-        <v>0.33037300177619894</v>
+        <v>0.38212927756653992</v>
       </c>
       <c r="M7" s="20">
         <f>SUM(J7:K7)</f>
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="N7" s="35">
         <f>M7/E7</f>
-        <v>0.369449378330373</v>
+        <v>0.42775665399239543</v>
       </c>
       <c r="O7">
         <f>SUM(O3:O5)</f>
-        <v>355</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1817,17 +1818,18 @@
         <v>5</v>
       </c>
       <c r="B8" s="28">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$472</f>
-        <v>14</v>
-      </c>
+        <f>'[1]Antibody-POST'!$J$471</f>
+        <v>16</v>
+      </c>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:15" ht="16" thickBot="1">
       <c r="A9" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="31">
-        <f>'[1]Antibody-POST 1st vs 2nd Abs'!$G$476</f>
-        <v>152</v>
+        <f>'[1]Antibody-POST'!$J$475</f>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickBot="1">
@@ -1855,7 +1857,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="28">
-        <f>'[1]Organisms- POST'!$E$145</f>
+        <f>'[1]Organisms- POST'!$H$145</f>
         <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1863,15 +1865,15 @@
       </c>
       <c r="E12" s="36">
         <f>'Semantic correctness'!E3</f>
-        <v>0.96744186046511627</v>
+        <v>0.95928753180661575</v>
       </c>
       <c r="F12" s="36">
         <f>'Syntactic correctness'!F3</f>
-        <v>0.64651162790697669</v>
+        <v>0.5750636132315522</v>
       </c>
       <c r="G12" s="36">
         <f>O3/E3</f>
-        <v>0.61395348837209307</v>
+        <v>0.53435114503816794</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1879,7 +1881,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="28">
-        <f>'[1]Organisms- POST'!$E$152</f>
+        <f>'[1]Organisms- POST'!$H$152</f>
         <v>139</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1903,11 +1905,11 @@
         <v>11</v>
       </c>
       <c r="B14" s="28">
-        <f>'[1]Organisms- POST'!$E$149</f>
+        <f>'[1]Organisms- POST'!$H$149</f>
         <v>84</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E14" s="36">
         <f>'Semantic correctness'!E5</f>
@@ -1935,15 +1937,15 @@
       </c>
       <c r="E15" s="37">
         <f>'Semantic correctness'!E7</f>
-        <v>0.96092362344582594</v>
+        <v>0.95437262357414454</v>
       </c>
       <c r="F15" s="37">
         <f>'Syntactic correctness'!F6</f>
-        <v>0.66962699822380112</v>
+        <v>0.61787072243346008</v>
       </c>
       <c r="G15" s="37">
         <f>O7/E7</f>
-        <v>0.63055062166962694</v>
+        <v>0.57224334600760451</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1951,7 +1953,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="28">
-        <f>'[1]Organisms- POST'!$G$145</f>
+        <f>'[1]Organisms- POST'!$J$145</f>
         <v>7</v>
       </c>
     </row>
@@ -1960,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="31">
-        <f>'[1]Organisms- POST'!$G$149</f>
+        <f>'[1]Organisms- POST'!$J$149</f>
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1991,19 +1993,19 @@
       </c>
       <c r="E19">
         <f>I3</f>
-        <v>416</v>
+        <v>377</v>
       </c>
       <c r="F19">
         <f>'Syntactic correctness'!E3</f>
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="G19">
         <f>O3</f>
-        <v>264</v>
+        <v>210</v>
       </c>
       <c r="H19">
         <f>E3</f>
-        <v>430</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2011,7 +2013,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="28">
-        <f>'[1]Software- POST C v NC'!$E$106</f>
+        <f>'[1]Software- POST C v NC'!$H$106</f>
         <v>78</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2039,11 +2041,11 @@
         <v>13</v>
       </c>
       <c r="B21" s="28">
-        <f>'[1]Software- POST C v NC'!$E$113</f>
+        <f>'[1]Software- POST C v NC'!$H$113</f>
         <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E21">
         <f>I5</f>
@@ -2067,7 +2069,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="28">
-        <f>'[1]Software- POST C v NC'!$E$110</f>
+        <f>'[1]Software- POST C v NC'!$H$110</f>
         <v>22</v>
       </c>
       <c r="D22" s="23" t="s">
@@ -2075,19 +2077,19 @@
       </c>
       <c r="E22" s="23">
         <f>SUM(E19:E21)</f>
-        <v>541</v>
+        <v>502</v>
       </c>
       <c r="F22" s="23">
         <f>'Syntactic correctness'!E6</f>
-        <v>377</v>
+        <v>325</v>
       </c>
       <c r="G22" s="23">
         <f>SUM(G19:G21)</f>
-        <v>355</v>
+        <v>301</v>
       </c>
       <c r="H22" s="23">
         <f>SUM(H19:H21)</f>
-        <v>563</v>
+        <v>526</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2098,25 +2100,16 @@
         <f>B20-B24</f>
         <v>77</v>
       </c>
-      <c r="E23" s="3">
-        <f>E22/$H$22</f>
-        <v>0.96092362344582594</v>
-      </c>
-      <c r="F23" s="3">
-        <f>F22/$H$22</f>
-        <v>0.66962699822380112</v>
-      </c>
-      <c r="G23" s="3">
-        <f>G22/$H$22</f>
-        <v>0.63055062166962694</v>
-      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="28">
-        <f>'[1]Software- POST C v NC'!$G$106</f>
+        <f>'[1]Software- POST C v NC'!$J$106</f>
         <v>1</v>
       </c>
     </row>
@@ -2125,7 +2118,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="31">
-        <f>'[1]Software- POST C v NC'!$G$110</f>
+        <f>'[1]Software- POST C v NC'!$J$110</f>
         <v>26</v>
       </c>
     </row>
@@ -2179,23 +2172,23 @@
       </c>
       <c r="B3">
         <f>'Data summary'!B7</f>
-        <v>416</v>
+        <v>377</v>
       </c>
       <c r="C3">
         <f>'Data summary'!B8</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <f>'Data summary'!B4</f>
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="E3" s="3">
         <f>B3/D3</f>
-        <v>0.96744186046511627</v>
+        <v>0.95928753180661575</v>
       </c>
       <c r="F3" s="3">
         <f>C3/D3</f>
-        <v>3.255813953488372E-2</v>
+        <v>4.0712468193384227E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2258,23 +2251,23 @@
       </c>
       <c r="B7">
         <f>SUM(B3:B5)</f>
-        <v>541</v>
+        <v>502</v>
       </c>
       <c r="C7">
         <f>SUM(C3:C5)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <f>SUM(D3:D5)</f>
-        <v>563</v>
+        <v>526</v>
       </c>
       <c r="E7" s="7">
         <f>B7/D7</f>
-        <v>0.96092362344582594</v>
+        <v>0.95437262357414454</v>
       </c>
       <c r="F7" s="7">
         <f>C7/D7</f>
-        <v>3.9076376554174071E-2</v>
+        <v>4.5627376425855515E-2</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -2301,15 +2294,15 @@
       </c>
       <c r="B11" s="9">
         <f t="shared" ref="B11:C13" si="1">C3</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="9">
         <f t="shared" si="1"/>
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="D11" s="10">
         <f>F3</f>
-        <v>3.255813953488372E-2</v>
+        <v>4.0712468193384227E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2352,11 +2345,11 @@
       </c>
       <c r="B14" s="13">
         <f>SUM(B11:B13)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C14" s="13">
         <f>SUM(C11:C13)</f>
-        <v>563</v>
+        <v>526</v>
       </c>
       <c r="D14" s="14">
         <v>4.6181172291296625E-2</v>
@@ -2412,23 +2405,23 @@
       </c>
       <c r="B3" s="9">
         <f>'Data summary'!K3</f>
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C3" s="9">
         <f>'Data summary'!E3</f>
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="D3" s="10">
         <f>B3/C3</f>
-        <v>0.35348837209302325</v>
+        <v>0.42493638676844786</v>
       </c>
       <c r="E3">
         <f>C3-B3</f>
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="F3" s="3">
         <f>E3/C3</f>
-        <v>0.64651162790697669</v>
+        <v>0.5750636132315522</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2487,23 +2480,23 @@
       </c>
       <c r="B6" s="13">
         <f>SUM(B3:B5)</f>
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="C6" s="13">
         <f>SUM(C3:C5)</f>
-        <v>563</v>
+        <v>526</v>
       </c>
       <c r="D6" s="14">
         <f>B6/C6</f>
-        <v>0.33037300177619894</v>
+        <v>0.38212927756653992</v>
       </c>
       <c r="E6">
         <f>C6-B6</f>
-        <v>377</v>
+        <v>325</v>
       </c>
       <c r="F6" s="3">
         <f>E6/C6</f>
-        <v>0.66962699822380112</v>
+        <v>0.61787072243346008</v>
       </c>
     </row>
   </sheetData>
@@ -2563,27 +2556,27 @@
       </c>
       <c r="B3">
         <f>'Data summary'!E3</f>
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="C3">
         <f>'Data summary'!I3</f>
-        <v>416</v>
+        <v>377</v>
       </c>
       <c r="D3">
         <f>'Data summary'!J3</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <f>'Data summary'!K3</f>
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="F3">
         <f>SUM(D3:E3)</f>
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="G3" s="3">
         <f>F3/B3</f>
-        <v>0.38604651162790699</v>
+        <v>0.46564885496183206</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2653,27 +2646,27 @@
       </c>
       <c r="B7" s="23">
         <f>'Data summary'!E7</f>
-        <v>563</v>
+        <v>526</v>
       </c>
       <c r="C7" s="23">
         <f>'Data summary'!I7</f>
-        <v>541</v>
+        <v>502</v>
       </c>
       <c r="D7" s="23">
         <f>'Data summary'!J7</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" s="23">
         <f>'Data summary'!K7</f>
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="F7" s="23">
         <f>SUM(D7:E7)</f>
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="G7" s="24">
         <f>F7/B7</f>
-        <v>0.369449378330373</v>
+        <v>0.42775665399239543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizing dataset for sharing.
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
+++ b/DataRe-Analysis/SummaryCalculations_RII_Paper_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="23840" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="23840" windowHeight="15740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>Total count</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Tools</t>
+  </si>
+  <si>
+    <t>Correct synatx</t>
   </si>
 </sst>
 </file>
@@ -435,9 +438,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="184">
+  <cellStyleXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -673,7 +686,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="184">
+  <cellStyles count="194">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -765,6 +778,11 @@
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -856,6 +874,11 @@
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -907,13 +930,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.959287531806616</c:v>
+                  <c:v>0.962703962703963</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.575063613231552</c:v>
+                  <c:v>0.629370629370629</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.534351145038168</c:v>
+                  <c:v>0.592074592074592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,7 +1097,7 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1118,23 +1141,23 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="471">
-          <cell r="H471">
-            <v>393</v>
+          <cell r="G471">
+            <v>429</v>
           </cell>
-          <cell r="J471">
+          <cell r="I471">
             <v>16</v>
           </cell>
         </row>
         <row r="475">
-          <cell r="H475">
+          <cell r="G475">
             <v>36</v>
           </cell>
-          <cell r="J475">
-            <v>167</v>
+          <cell r="I475">
+            <v>159</v>
           </cell>
         </row>
         <row r="478">
-          <cell r="H478">
+          <cell r="G478">
             <v>465</v>
           </cell>
         </row>
@@ -1142,23 +1165,23 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="145">
-          <cell r="H145">
+          <cell r="G145">
             <v>55</v>
           </cell>
-          <cell r="J145">
+          <cell r="I145">
             <v>7</v>
           </cell>
         </row>
         <row r="149">
-          <cell r="H149">
+          <cell r="G149">
             <v>84</v>
           </cell>
-          <cell r="J149">
+          <cell r="I149">
             <v>8</v>
           </cell>
         </row>
         <row r="152">
-          <cell r="H152">
+          <cell r="G152">
             <v>139</v>
           </cell>
         </row>
@@ -1166,23 +1189,23 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="106">
-          <cell r="H106">
+          <cell r="G106">
             <v>78</v>
           </cell>
-          <cell r="J106">
+          <cell r="I106">
             <v>1</v>
           </cell>
         </row>
         <row r="110">
-          <cell r="H110">
+          <cell r="G110">
             <v>22</v>
           </cell>
-          <cell r="J110">
+          <cell r="I110">
             <v>26</v>
           </cell>
         </row>
         <row r="113">
-          <cell r="H113">
+          <cell r="G113">
             <v>101</v>
           </cell>
         </row>
@@ -1518,21 +1541,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="47" thickBot="1">
+    <row r="1" spans="1:16" ht="47" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -1540,7 +1565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="46" thickBot="1">
+    <row r="2" spans="1:16" ht="46" thickBot="1">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -1568,19 +1593,22 @@
         <v>28</v>
       </c>
       <c r="L2" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="N2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="P2" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1">
+    <row r="3" spans="1:16" s="2" customFormat="1">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -1589,15 +1617,15 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f>'[1]Antibody-POST'!$H$471</f>
-        <v>393</v>
+        <f>'[1]Antibody-POST'!$G$471</f>
+        <v>429</v>
       </c>
       <c r="F3">
-        <f>'[1]Antibody-POST'!$H$478</f>
+        <f>'[1]Antibody-POST'!$G$478</f>
         <v>465</v>
       </c>
       <c r="G3">
-        <f>'[1]Antibody-POST'!$H$475</f>
+        <f>'[1]Antibody-POST'!$G$475</f>
         <v>36</v>
       </c>
       <c r="H3" s="3">
@@ -1606,54 +1634,58 @@
       </c>
       <c r="I3">
         <f>E3-J3</f>
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="J3">
-        <f>'[1]Antibody-POST'!$J$471</f>
+        <f>'[1]Antibody-POST'!$I$471</f>
         <v>16</v>
       </c>
       <c r="K3">
-        <f>'[1]Antibody-POST'!$J$475</f>
-        <v>167</v>
-      </c>
-      <c r="L3" s="3">
+        <f>'[1]Antibody-POST'!$I$475</f>
+        <v>159</v>
+      </c>
+      <c r="L3">
+        <f>E3-K3</f>
+        <v>270</v>
+      </c>
+      <c r="M3" s="3">
         <f>K3/E3</f>
-        <v>0.42493638676844786</v>
-      </c>
-      <c r="M3">
+        <v>0.37062937062937062</v>
+      </c>
+      <c r="N3">
         <f>SUM(J3:K3)</f>
-        <v>183</v>
-      </c>
-      <c r="N3" s="3">
-        <f>M3/E3</f>
-        <v>0.46564885496183206</v>
-      </c>
-      <c r="O3" s="2">
+        <v>175</v>
+      </c>
+      <c r="O3" s="3">
+        <f>N3/E3</f>
+        <v>0.40792540792540793</v>
+      </c>
+      <c r="P3" s="2">
         <f>E3-J3-K3</f>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="28">
-        <f>'[1]Antibody-POST'!$H$471</f>
-        <v>393</v>
+        <f>'[1]Antibody-POST'!$G$471</f>
+        <v>429</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4">
-        <f>'[1]Organisms- POST'!$H$145</f>
+        <f>'[1]Organisms- POST'!$G$145</f>
         <v>55</v>
       </c>
       <c r="F4">
-        <f>'[1]Organisms- POST'!$H$152</f>
+        <f>'[1]Organisms- POST'!$G$152</f>
         <v>139</v>
       </c>
       <c r="G4">
-        <f>'[1]Organisms- POST'!$H$149</f>
+        <f>'[1]Organisms- POST'!$G$149</f>
         <v>84</v>
       </c>
       <c r="H4" s="3">
@@ -1665,51 +1697,55 @@
         <v>48</v>
       </c>
       <c r="J4">
-        <f>'[1]Organisms- POST'!$J$145</f>
+        <f>'[1]Organisms- POST'!$I$145</f>
         <v>7</v>
       </c>
       <c r="K4">
-        <f>'[1]Organisms- POST'!$J$149</f>
+        <f>'[1]Organisms- POST'!$I$149</f>
         <v>8</v>
       </c>
-      <c r="L4" s="3">
-        <f t="shared" ref="L4:L7" si="0">K4/E4</f>
+      <c r="L4">
+        <f>E4-K4</f>
+        <v>47</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M7" si="0">K4/E4</f>
         <v>0.14545454545454545</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f>SUM(J4:K4)</f>
         <v>15</v>
       </c>
-      <c r="N4" s="3">
-        <f>M4/E4</f>
+      <c r="O4" s="3">
+        <f>N4/E4</f>
         <v>0.27272727272727271</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <f>E4-J4-K4</f>
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="28">
-        <f>'[1]Antibody-POST'!$H$478</f>
+        <f>'[1]Antibody-POST'!$G$478</f>
         <v>465</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E5">
-        <f>'[1]Software- POST C v NC'!$H$106</f>
+        <f>'[1]Software- POST C v NC'!$G$106</f>
         <v>78</v>
       </c>
       <c r="F5">
-        <f>'[1]Software- POST C v NC'!$H$113</f>
+        <f>'[1]Software- POST C v NC'!$G$113</f>
         <v>101</v>
       </c>
       <c r="G5">
-        <f>'[1]Software- POST C v NC'!$H$110</f>
+        <f>'[1]Software- POST C v NC'!$G$110</f>
         <v>22</v>
       </c>
       <c r="H5" s="3">
@@ -1721,56 +1757,60 @@
         <v>77</v>
       </c>
       <c r="J5">
-        <f>'[1]Software- POST C v NC'!$J$106</f>
+        <f>'[1]Software- POST C v NC'!$I$106</f>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>'[1]Software- POST C v NC'!$J$110</f>
+        <f>'[1]Software- POST C v NC'!$I$110</f>
         <v>26</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
+        <f>E5-K5</f>
+        <v>52</v>
+      </c>
+      <c r="M5" s="3">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f>SUM(J5:K5)</f>
         <v>27</v>
       </c>
-      <c r="N5" s="3">
-        <f>M5/E5</f>
+      <c r="O5" s="3">
+        <f>N5/E5</f>
         <v>0.34615384615384615</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <f>E5-J5-K5</f>
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="28">
-        <f>'[1]Antibody-POST'!$H$475</f>
+        <f>'[1]Antibody-POST'!$G$475</f>
         <v>36</v>
       </c>
       <c r="D6" s="1"/>
       <c r="H6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="28">
         <f>B4-B8</f>
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="23">
         <f>SUM(E3:E5)</f>
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="F7" s="23">
         <f>SUM(F3:F5)</f>
@@ -1786,7 +1826,7 @@
       </c>
       <c r="I7" s="23">
         <f>SUM(I3:I5)</f>
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="J7" s="23">
         <f>SUM(J3:J5)</f>
@@ -1794,50 +1834,54 @@
       </c>
       <c r="K7" s="23">
         <f>SUM(K3:K5)</f>
-        <v>201</v>
-      </c>
-      <c r="L7" s="24">
+        <v>193</v>
+      </c>
+      <c r="L7" s="23">
+        <f>SUM(L3:L5)</f>
+        <v>369</v>
+      </c>
+      <c r="M7" s="24">
         <f t="shared" si="0"/>
-        <v>0.38212927756653992</v>
-      </c>
-      <c r="M7" s="20">
+        <v>0.34341637010676157</v>
+      </c>
+      <c r="N7" s="20">
         <f>SUM(J7:K7)</f>
-        <v>225</v>
-      </c>
-      <c r="N7" s="35">
-        <f>M7/E7</f>
-        <v>0.42775665399239543</v>
-      </c>
-      <c r="O7">
-        <f>SUM(O3:O5)</f>
-        <v>301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="O7" s="35">
+        <f>N7/E7</f>
+        <v>0.38612099644128112</v>
+      </c>
+      <c r="P7" s="20">
+        <f>SUM(P3:P5)</f>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="28">
-        <f>'[1]Antibody-POST'!$J$471</f>
+        <f>'[1]Antibody-POST'!$I$471</f>
         <v>16</v>
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="16" thickBot="1">
+    <row r="9" spans="1:16" ht="16" thickBot="1">
       <c r="A9" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="31">
-        <f>'[1]Antibody-POST'!$J$475</f>
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="16" thickBot="1">
+        <f>'[1]Antibody-POST'!$I$475</f>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16" thickBot="1">
       <c r="D10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="46" thickBot="1">
+    <row r="11" spans="1:16" ht="46" thickBot="1">
       <c r="A11" s="32" t="s">
         <v>8</v>
       </c>
@@ -1852,79 +1896,79 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" s="27" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="28">
-        <f>'[1]Organisms- POST'!$H$145</f>
+        <f>'[1]Organisms- POST'!$G$145</f>
         <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="36">
-        <f>'Semantic correctness'!E3</f>
-        <v>0.95928753180661575</v>
+        <f>I3/E3</f>
+        <v>0.96270396270396275</v>
       </c>
       <c r="F12" s="36">
-        <f>'Syntactic correctness'!F3</f>
-        <v>0.5750636132315522</v>
+        <f>L3/E3</f>
+        <v>0.62937062937062938</v>
       </c>
       <c r="G12" s="36">
-        <f>O3/E3</f>
-        <v>0.53435114503816794</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <f>P3/E3</f>
+        <v>0.59207459207459212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="28">
-        <f>'[1]Organisms- POST'!$H$152</f>
+        <f>'[1]Organisms- POST'!$G$152</f>
         <v>139</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="36">
-        <f>'Semantic correctness'!E4</f>
+        <f>I4/E4</f>
         <v>0.87272727272727268</v>
       </c>
       <c r="F13" s="36">
-        <f>'Syntactic correctness'!F4</f>
+        <f>L4/E4</f>
         <v>0.8545454545454545</v>
       </c>
       <c r="G13" s="36">
-        <f>O4/E4</f>
+        <f>P4/E4</f>
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="28">
-        <f>'[1]Organisms- POST'!$H$149</f>
+        <f>'[1]Organisms- POST'!$G$149</f>
         <v>84</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E14" s="36">
-        <f>'Semantic correctness'!E5</f>
+        <f>I5/E5</f>
         <v>0.98717948717948723</v>
       </c>
       <c r="F14" s="36">
-        <f>'Syntactic correctness'!F5</f>
+        <f>L5/E5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="G14" s="36">
-        <f>O5/E5</f>
+        <f>P5/E5</f>
         <v>0.65384615384615385</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
@@ -1936,24 +1980,24 @@
         <v>18</v>
       </c>
       <c r="E15" s="37">
-        <f>'Semantic correctness'!E7</f>
-        <v>0.95437262357414454</v>
+        <f>I7/E7</f>
+        <v>0.95729537366548045</v>
       </c>
       <c r="F15" s="37">
-        <f>'Syntactic correctness'!F6</f>
-        <v>0.61787072243346008</v>
+        <f>L7/E7</f>
+        <v>0.65658362989323849</v>
       </c>
       <c r="G15" s="37">
-        <f>O7/E7</f>
-        <v>0.57224334600760451</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <f>P7/E7</f>
+        <v>0.61387900355871883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="28">
-        <f>'[1]Organisms- POST'!$J$145</f>
+        <f>'[1]Organisms- POST'!$I$145</f>
         <v>7</v>
       </c>
     </row>
@@ -1962,7 +2006,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="31">
-        <f>'[1]Organisms- POST'!$J$149</f>
+        <f>'[1]Organisms- POST'!$I$149</f>
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1993,19 +2037,19 @@
       </c>
       <c r="E19">
         <f>I3</f>
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="F19">
         <f>'Syntactic correctness'!E3</f>
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="G19">
-        <f>O3</f>
-        <v>210</v>
+        <f>P3</f>
+        <v>254</v>
       </c>
       <c r="H19">
         <f>E3</f>
-        <v>393</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2013,7 +2057,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="28">
-        <f>'[1]Software- POST C v NC'!$H$106</f>
+        <f>'[1]Software- POST C v NC'!$G$106</f>
         <v>78</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2028,7 +2072,7 @@
         <v>47</v>
       </c>
       <c r="G20">
-        <f>O4</f>
+        <f>P4</f>
         <v>40</v>
       </c>
       <c r="H20">
@@ -2041,7 +2085,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="28">
-        <f>'[1]Software- POST C v NC'!$H$113</f>
+        <f>'[1]Software- POST C v NC'!$G$113</f>
         <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -2056,7 +2100,7 @@
         <v>52</v>
       </c>
       <c r="G21">
-        <f>O5</f>
+        <f>P5</f>
         <v>51</v>
       </c>
       <c r="H21">
@@ -2069,7 +2113,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="28">
-        <f>'[1]Software- POST C v NC'!$H$110</f>
+        <f>'[1]Software- POST C v NC'!$G$110</f>
         <v>22</v>
       </c>
       <c r="D22" s="23" t="s">
@@ -2077,19 +2121,19 @@
       </c>
       <c r="E22" s="23">
         <f>SUM(E19:E21)</f>
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="F22" s="23">
         <f>'Syntactic correctness'!E6</f>
-        <v>325</v>
+        <v>369</v>
       </c>
       <c r="G22" s="23">
         <f>SUM(G19:G21)</f>
-        <v>301</v>
+        <v>345</v>
       </c>
       <c r="H22" s="23">
         <f>SUM(H19:H21)</f>
-        <v>526</v>
+        <v>562</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2109,7 +2153,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="28">
-        <f>'[1]Software- POST C v NC'!$J$106</f>
+        <f>'[1]Software- POST C v NC'!$I$106</f>
         <v>1</v>
       </c>
     </row>
@@ -2118,7 +2162,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="31">
-        <f>'[1]Software- POST C v NC'!$J$110</f>
+        <f>'[1]Software- POST C v NC'!$I$110</f>
         <v>26</v>
       </c>
     </row>
@@ -2138,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2172,7 +2216,7 @@
       </c>
       <c r="B3">
         <f>'Data summary'!B7</f>
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="C3">
         <f>'Data summary'!B8</f>
@@ -2180,15 +2224,15 @@
       </c>
       <c r="D3">
         <f>'Data summary'!B4</f>
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="E3" s="3">
         <f>B3/D3</f>
-        <v>0.95928753180661575</v>
+        <v>0.96270396270396275</v>
       </c>
       <c r="F3" s="3">
         <f>C3/D3</f>
-        <v>4.0712468193384227E-2</v>
+        <v>3.7296037296037296E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2251,7 +2295,7 @@
       </c>
       <c r="B7">
         <f>SUM(B3:B5)</f>
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="C7">
         <f>SUM(C3:C5)</f>
@@ -2259,15 +2303,15 @@
       </c>
       <c r="D7">
         <f>SUM(D3:D5)</f>
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="E7" s="7">
         <f>B7/D7</f>
-        <v>0.95437262357414454</v>
+        <v>0.95729537366548045</v>
       </c>
       <c r="F7" s="7">
         <f>C7/D7</f>
-        <v>4.5627376425855515E-2</v>
+        <v>4.2704626334519574E-2</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -2298,11 +2342,11 @@
       </c>
       <c r="C11" s="9">
         <f t="shared" si="1"/>
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="D11" s="10">
         <f>F3</f>
-        <v>4.0712468193384227E-2</v>
+        <v>3.7296037296037296E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2349,7 +2393,7 @@
       </c>
       <c r="C14" s="13">
         <f>SUM(C11:C13)</f>
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="D14" s="14">
         <v>4.6181172291296625E-2</v>
@@ -2371,7 +2415,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F3:F6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2405,23 +2449,23 @@
       </c>
       <c r="B3" s="9">
         <f>'Data summary'!K3</f>
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C3" s="9">
         <f>'Data summary'!E3</f>
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="D3" s="10">
         <f>B3/C3</f>
-        <v>0.42493638676844786</v>
+        <v>0.37062937062937062</v>
       </c>
       <c r="E3">
         <f>C3-B3</f>
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="F3" s="3">
         <f>E3/C3</f>
-        <v>0.5750636132315522</v>
+        <v>0.62937062937062938</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2480,23 +2524,23 @@
       </c>
       <c r="B6" s="13">
         <f>SUM(B3:B5)</f>
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C6" s="13">
         <f>SUM(C3:C5)</f>
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="D6" s="14">
         <f>B6/C6</f>
-        <v>0.38212927756653992</v>
+        <v>0.34341637010676157</v>
       </c>
       <c r="E6">
         <f>C6-B6</f>
-        <v>325</v>
+        <v>369</v>
       </c>
       <c r="F6" s="3">
         <f>E6/C6</f>
-        <v>0.61787072243346008</v>
+        <v>0.65658362989323849</v>
       </c>
     </row>
   </sheetData>
@@ -2556,11 +2600,11 @@
       </c>
       <c r="B3">
         <f>'Data summary'!E3</f>
-        <v>393</v>
+        <v>429</v>
       </c>
       <c r="C3">
         <f>'Data summary'!I3</f>
-        <v>377</v>
+        <v>413</v>
       </c>
       <c r="D3">
         <f>'Data summary'!J3</f>
@@ -2568,15 +2612,15 @@
       </c>
       <c r="E3">
         <f>'Data summary'!K3</f>
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F3">
         <f>SUM(D3:E3)</f>
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G3" s="3">
         <f>F3/B3</f>
-        <v>0.46564885496183206</v>
+        <v>0.40792540792540793</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2646,11 +2690,11 @@
       </c>
       <c r="B7" s="23">
         <f>'Data summary'!E7</f>
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="C7" s="23">
         <f>'Data summary'!I7</f>
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="D7" s="23">
         <f>'Data summary'!J7</f>
@@ -2658,15 +2702,15 @@
       </c>
       <c r="E7" s="23">
         <f>'Data summary'!K7</f>
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F7" s="23">
         <f>SUM(D7:E7)</f>
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G7" s="24">
         <f>F7/B7</f>
-        <v>0.42775665399239543</v>
+        <v>0.38612099644128112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>